<commit_message>
Include imported electricity emissions
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
+++ b/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-minnesota\InputData\ctrl-settings\BIEfIE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="22035" windowHeight="11835"/>
   </bookViews>
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,6 +109,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -151,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,7 +194,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,49 +407,49 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -459,21 +467,23 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to MN data plus turning on include imported elec emissions
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
+++ b/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\ctrl-settings\BIEfIE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78224D2-2C5A-487F-9787-0ACFD43B41F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="22035" windowHeight="11835"/>
+    <workbookView xWindow="4740" yWindow="1650" windowWidth="21000" windowHeight="14430" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -53,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,6 +110,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -151,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,9 +193,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +245,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,10 +437,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -453,13 +496,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -473,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated imported elec and fuels
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
+++ b/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Minnesota\MN_mod\InputData\ctrl-settings\BIEfIE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E314CDA-133E-4C5E-84E4-48A70D22BC99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="22035" windowHeight="11835"/>
+    <workbookView xWindow="465" yWindow="525" windowWidth="21540" windowHeight="16710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -53,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,6 +110,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -151,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,9 +193,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +245,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,10 +437,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -453,13 +496,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -473,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
turn on imported emissions
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
+++ b/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/ctrl-settings/biefie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Minnesota\MN-EPS\InputData\ctrl-settings\BIEfIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611D035E-B30F-3943-8580-0E58F028C670}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CC4296-C87C-463A-B637-38F4899E19EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="22040" windowHeight="11840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="950" windowWidth="20230" windowHeight="13450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -441,11 +441,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -453,42 +453,42 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -506,21 +506,23 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>